<commit_message>
Updated BOM and readme
</commit_message>
<xml_diff>
--- a/Proto-Pi-BOM.xlsx
+++ b/Proto-Pi-BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parke\Documents\GitHub\Proto-Pi-Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8893DBE-F459-48A1-B151-30535CD1776D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EB0605-4826-4E75-84CA-9033D6877D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15990" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Line Item</t>
   </si>
@@ -43,9 +43,6 @@
     <t>JP1</t>
   </si>
   <si>
-    <t>RASBERRYPI_IDC</t>
-  </si>
-  <si>
     <t>D1, D2, D3</t>
   </si>
   <si>
@@ -73,18 +70,12 @@
     <t>CONN1</t>
   </si>
   <si>
-    <t>CON-HEADER-1X25</t>
-  </si>
-  <si>
     <t>CONN2, CONN3</t>
   </si>
   <si>
     <t>JST_SH4</t>
   </si>
   <si>
-    <t>CON-STEMMA_I2C_QT</t>
-  </si>
-  <si>
     <t>IC2</t>
   </si>
   <si>
@@ -113,13 +104,58 @@
   </si>
   <si>
     <t>771-PCA9685PW</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>755-SML-D12P8WT86C</t>
+  </si>
+  <si>
+    <t>SML-D12P8WT86C</t>
+  </si>
+  <si>
+    <t>10Kohm</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>MCP3008-I/SL</t>
+  </si>
+  <si>
+    <t>579-MCP3008-I/SL</t>
+  </si>
+  <si>
+    <t>4208</t>
+  </si>
+  <si>
+    <t>485-4208</t>
+  </si>
+  <si>
+    <t>2x13 ICD Connetor</t>
+  </si>
+  <si>
+    <t>SOIC-16</t>
+  </si>
+  <si>
+    <t>2.54MM MALE PIN HEADER</t>
+  </si>
+  <si>
+    <t>2.54mm 2X13 Female IDC Connector</t>
+  </si>
+  <si>
+    <t>CONNECTOR</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +286,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -552,7 +596,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -595,12 +639,24 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -634,6 +690,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -957,15 +1014,16 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -990,143 +1048,214 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
+      <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
         <v>603</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
         <v>402</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>603</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>603</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3">
+        <v>603</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
-        <v>603</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
+      <c r="E6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
-        <v>15</v>
+      <c r="E7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" display="https://www.mouser.com/ProductDetail/755-SML-D12P8WT86C" xr:uid="{1C69C5B1-D387-4A64-A1A0-717B8E5FBA4F}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{23FB2178-1DF0-4230-964A-BF5206525BFC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E9" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>